<commit_message>
Fix cases to iterate again on 3x3 case for higher accuracy
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/FullQRTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/FullQRTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="1875" windowWidth="18915" windowHeight="8775" activeTab="1"/>
+    <workbookView xWindow="60" yWindow="1875" windowWidth="18915" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="Full 4x4" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="90">
   <si>
     <t>#1</t>
   </si>
@@ -300,16 +300,13 @@
     <t>Deflated to 3x3 case</t>
   </si>
   <si>
-    <t>Deflated to 2x2 case</t>
-  </si>
-  <si>
     <t>Delta=</t>
   </si>
   <si>
-    <t>Both complex root, Done.</t>
+    <t>G2*G1=</t>
   </si>
   <si>
-    <t>G2*G1=</t>
+    <t>Deflated to 2x2. Both complex root, Done.</t>
   </si>
 </sst>
 </file>
@@ -359,13 +356,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -670,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV192"/>
+  <dimension ref="A1:AV207"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="AF173" sqref="AF173:AN176"/>
+    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -682,6 +682,7 @@
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
     <col min="32" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -6473,7 +6474,7 @@
       <c r="AD167" s="1"/>
       <c r="AE167" s="1"/>
       <c r="AF167" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AG167" s="1"/>
       <c r="AH167" s="1"/>
@@ -6929,12 +6930,12 @@
         <v>-13.000683863926154</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:35">
       <c r="A178" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:35">
       <c r="A179">
         <v>4</v>
       </c>
@@ -6942,7 +6943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:35">
       <c r="A180">
         <f>A173+M165</f>
         <v>-10.029677613025422</v>
@@ -6951,7 +6952,7 @@
         <f t="shared" ref="B180:D180" si="81">B173</f>
         <v>-7.5286908111153901</v>
       </c>
-      <c r="C180" s="2">
+      <c r="C180">
         <f t="shared" si="81"/>
         <v>-3.8347798670194888</v>
       </c>
@@ -6960,10 +6961,16 @@
         <v>3.3291102244277555</v>
       </c>
       <c r="F180" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10">
+        <v>86</v>
+      </c>
+      <c r="L180" t="s">
+        <v>74</v>
+      </c>
+      <c r="M180">
+        <v>12.587508723557301</v>
+      </c>
+    </row>
+    <row r="181" spans="1:35">
       <c r="A181">
         <f t="shared" ref="A181" si="82">A174</f>
         <v>7.3698359137508982</v>
@@ -6972,7 +6979,7 @@
         <f>B174+M165</f>
         <v>1.5266632516900671</v>
       </c>
-      <c r="C181" s="2">
+      <c r="C181">
         <f t="shared" ref="C181:D181" si="83">C174</f>
         <v>12.590370584930435</v>
       </c>
@@ -6996,16 +7003,16 @@
         <v>-8.5030143613353548</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
-      <c r="A182" s="2">
+    <row r="182" spans="1:35">
+      <c r="A182">
         <f t="shared" ref="A182:B182" si="84">A175</f>
         <v>2.1207995017926617E-19</v>
       </c>
-      <c r="B182" s="2">
+      <c r="B182">
         <f t="shared" si="84"/>
         <v>-2.3781157270230822E-12</v>
       </c>
-      <c r="C182" s="2">
+      <c r="C182">
         <f>C175+M165</f>
         <v>12.587508723559308</v>
       </c>
@@ -7029,7 +7036,7 @@
         <v>40.173275685180123</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:35">
       <c r="A183" s="2">
         <f t="shared" ref="A183:C183" si="86">A176</f>
         <v>-2.0088544357291023E-23</v>
@@ -7047,100 +7054,666 @@
         <v>-0.41317514036883907</v>
       </c>
       <c r="I183" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J183">
         <f>J181*J181-4*J182</f>
         <v>-88.391849511645205</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
-      <c r="A185" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="187" spans="1:10">
-      <c r="A187" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="188" spans="1:10">
-      <c r="A188">
-        <v>4</v>
-      </c>
-      <c r="B188">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="189" spans="1:10">
-      <c r="A189">
-        <f>A180</f>
-        <v>-10.029677613025422</v>
-      </c>
-      <c r="B189">
-        <f t="shared" ref="B189:D189" si="87">B180</f>
+    <row r="184" spans="1:35">
+      <c r="F184" s="1"/>
+      <c r="G184" s="1"/>
+      <c r="H184" s="1"/>
+      <c r="I184" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J184" s="1"/>
+      <c r="K184" s="1"/>
+      <c r="L184" s="1"/>
+      <c r="M184" s="1"/>
+      <c r="N184" s="1"/>
+      <c r="O184" s="1"/>
+      <c r="P184" s="1"/>
+      <c r="Q184" s="1"/>
+      <c r="R184" s="1"/>
+      <c r="S184" s="1"/>
+      <c r="T184" s="1"/>
+      <c r="U184" s="1"/>
+      <c r="V184" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W184" s="1"/>
+      <c r="X184" s="1"/>
+      <c r="Y184" s="1"/>
+      <c r="Z184" s="1"/>
+      <c r="AA184" s="1"/>
+      <c r="AB184" s="1"/>
+      <c r="AC184" s="1"/>
+      <c r="AD184" s="1"/>
+      <c r="AE184" s="1"/>
+      <c r="AF184" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG184" s="1"/>
+      <c r="AH184" s="1"/>
+      <c r="AI184" s="1"/>
+    </row>
+    <row r="185" spans="1:35">
+      <c r="A185">
+        <f>A180-M180</f>
+        <v>-22.617186336582723</v>
+      </c>
+      <c r="B185">
+        <f t="shared" ref="B185:C185" si="87">B180</f>
         <v>-7.5286908111153901</v>
       </c>
-      <c r="C189">
+      <c r="C185">
         <f t="shared" si="87"/>
         <v>-3.8347798670194888</v>
       </c>
-      <c r="D189">
-        <f t="shared" si="87"/>
+      <c r="D185" s="2">
+        <f>D180</f>
         <v>3.3291102244277555</v>
       </c>
-    </row>
-    <row r="190" spans="1:10">
-      <c r="A190">
-        <f t="shared" ref="A190:D190" si="88">A181</f>
+      <c r="F185" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G185" s="1">
+        <f>SQRT(SUMPRODUCT(A185:A186,A185:A186))</f>
+        <v>23.787635426399923</v>
+      </c>
+      <c r="H185" s="1"/>
+      <c r="I185" s="1">
+        <f>G186</f>
+        <v>-0.95079590430757077</v>
+      </c>
+      <c r="J185" s="1">
+        <f>-G187</f>
+        <v>0.30981792774458483</v>
+      </c>
+      <c r="K185" s="1">
+        <v>0</v>
+      </c>
+      <c r="L185" s="1">
+        <v>0</v>
+      </c>
+      <c r="M185" s="1"/>
+      <c r="N185" s="1">
+        <f t="array" ref="N185:Q188">MMULT(I185:L188,A185:D188)</f>
+        <v>23.787635426399927</v>
+      </c>
+      <c r="O185" s="1">
+        <v>3.7314001648095751</v>
+      </c>
+      <c r="P185" s="1">
+        <v>7.5468155156427841</v>
+      </c>
+      <c r="Q185" s="1">
+        <v>-1.0826114754889664</v>
+      </c>
+      <c r="R185" s="1"/>
+      <c r="S185" s="1"/>
+      <c r="T185" s="1"/>
+      <c r="U185" s="1"/>
+      <c r="V185" s="1">
+        <v>1</v>
+      </c>
+      <c r="W185" s="1">
+        <v>0</v>
+      </c>
+      <c r="X185" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y185" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z185" s="1"/>
+      <c r="AA185" s="1">
+        <f t="array" ref="AA185:AD188">MMULT(V185:Y188,N185:Q188)</f>
+        <v>23.787635426399927</v>
+      </c>
+      <c r="AB185" s="1">
+        <v>3.7314001648095751</v>
+      </c>
+      <c r="AC185" s="1">
+        <v>7.5468155156427841</v>
+      </c>
+      <c r="AD185" s="1">
+        <v>-1.0826114754889664</v>
+      </c>
+      <c r="AE185" s="1"/>
+      <c r="AF185" s="1">
+        <f t="array" ref="AF185:AI188">MMULT(V185:Y188, I185:L188)</f>
+        <v>-0.95079590430757077</v>
+      </c>
+      <c r="AG185" s="1">
+        <v>0.30981792774458483</v>
+      </c>
+      <c r="AH185" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI185" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:35">
+      <c r="A186">
+        <f t="shared" ref="A186" si="88">A181</f>
         <v>7.3698359137508982</v>
       </c>
-      <c r="B190">
-        <f t="shared" si="88"/>
-        <v>1.5266632516900671</v>
-      </c>
-      <c r="C190">
-        <f t="shared" si="88"/>
+      <c r="B186">
+        <f>B181-M180</f>
+        <v>-11.060845471867234</v>
+      </c>
+      <c r="C186">
+        <f t="shared" ref="C186:D186" si="89">C181</f>
         <v>12.590370584930435</v>
       </c>
-      <c r="D190">
-        <f t="shared" si="88"/>
+      <c r="D186" s="2">
+        <f t="shared" si="89"/>
         <v>6.7223123789091437</v>
       </c>
-    </row>
-    <row r="191" spans="1:10">
-      <c r="A191">
-        <f t="shared" ref="A191:D191" si="89">A182</f>
+      <c r="F186" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G186" s="1">
+        <f>A185/G185</f>
+        <v>-0.95079590430757077</v>
+      </c>
+      <c r="H186" s="1"/>
+      <c r="I186" s="1">
+        <f>-J185</f>
+        <v>-0.30981792774458483</v>
+      </c>
+      <c r="J186" s="1">
+        <f>I185</f>
+        <v>-0.95079590430757077</v>
+      </c>
+      <c r="K186" s="1">
+        <v>0</v>
+      </c>
+      <c r="L186" s="1">
+        <v>0</v>
+      </c>
+      <c r="M186" s="1"/>
+      <c r="N186" s="1">
+        <v>0</v>
+      </c>
+      <c r="O186" s="1">
+        <v>12.849129958559773</v>
+      </c>
+      <c r="P186" s="1">
+        <v>-10.782789234109739</v>
+      </c>
+      <c r="Q186" s="1">
+        <v>-7.4229651083084134</v>
+      </c>
+      <c r="R186" s="1"/>
+      <c r="S186" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T186" s="1">
+        <f>SQRT(SUMPRODUCT(O186:O187,O186:O187))</f>
+        <v>12.849129958559773</v>
+      </c>
+      <c r="U186" s="1"/>
+      <c r="V186" s="1">
+        <v>0</v>
+      </c>
+      <c r="W186" s="1">
+        <f>T187</f>
+        <v>1</v>
+      </c>
+      <c r="X186" s="1">
+        <f>-T188</f>
+        <v>-1.8507990305124436E-13</v>
+      </c>
+      <c r="Y186" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z186" s="1"/>
+      <c r="AA186" s="1">
+        <v>-3.9251736618291318E-32</v>
+      </c>
+      <c r="AB186" s="1">
+        <v>12.849129958559773</v>
+      </c>
+      <c r="AC186" s="1">
+        <v>-10.782789234109739</v>
+      </c>
+      <c r="AD186" s="1">
+        <v>-7.4229651083099206</v>
+      </c>
+      <c r="AE186" s="1"/>
+      <c r="AF186" s="1">
+        <v>-0.30981792774458483</v>
+      </c>
+      <c r="AG186" s="1">
+        <v>-0.95079590430757077</v>
+      </c>
+      <c r="AH186" s="1">
+        <v>-1.8507990305124436E-13</v>
+      </c>
+      <c r="AI186" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:35">
+      <c r="A187">
+        <f t="shared" ref="A187:B187" si="90">A182</f>
         <v>2.1207995017926617E-19</v>
       </c>
-      <c r="B191">
-        <f t="shared" si="89"/>
+      <c r="B187">
+        <f t="shared" si="90"/>
         <v>-2.3781157270230822E-12</v>
       </c>
-      <c r="C191">
-        <f t="shared" si="89"/>
-        <v>12.587508723559308</v>
-      </c>
-      <c r="D191">
-        <f t="shared" si="89"/>
+      <c r="C187">
+        <f>C182-M180</f>
+        <v>2.007283228522283E-12</v>
+      </c>
+      <c r="D187" s="2">
+        <f t="shared" ref="D187:D188" si="91">D182</f>
         <v>8.1439702435957582</v>
       </c>
-    </row>
-    <row r="192" spans="1:10">
-      <c r="A192">
-        <f t="shared" ref="A192:D192" si="90">A183</f>
+      <c r="F187" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G187" s="1">
+        <f>-A186/G185</f>
+        <v>-0.30981792774458483</v>
+      </c>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1">
+        <v>0</v>
+      </c>
+      <c r="J187" s="1">
+        <v>0</v>
+      </c>
+      <c r="K187" s="1">
+        <v>1</v>
+      </c>
+      <c r="L187" s="1">
+        <v>0</v>
+      </c>
+      <c r="M187" s="1"/>
+      <c r="N187" s="1">
+        <v>2.1207995017926617E-19</v>
+      </c>
+      <c r="O187" s="1">
+        <v>-2.3781157270230822E-12</v>
+      </c>
+      <c r="P187" s="1">
+        <v>2.007283228522283E-12</v>
+      </c>
+      <c r="Q187" s="1">
+        <v>8.1439702435957582</v>
+      </c>
+      <c r="R187" s="1"/>
+      <c r="S187" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T187" s="1">
+        <f>O186/T186</f>
+        <v>1</v>
+      </c>
+      <c r="U187" s="1"/>
+      <c r="V187" s="1">
+        <v>0</v>
+      </c>
+      <c r="W187" s="1">
+        <f>-X186</f>
+        <v>1.8507990305124436E-13</v>
+      </c>
+      <c r="X187" s="1">
+        <f>W186</f>
+        <v>1</v>
+      </c>
+      <c r="Y187" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z187" s="1"/>
+      <c r="AA187" s="1">
+        <v>2.1207995017926617E-19</v>
+      </c>
+      <c r="AB187" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC187" s="1">
+        <v>1.160564245125121E-14</v>
+      </c>
+      <c r="AD187" s="1">
+        <v>8.143970243594385</v>
+      </c>
+      <c r="AE187" s="1"/>
+      <c r="AF187" s="1">
+        <v>-5.7341072030505196E-14</v>
+      </c>
+      <c r="AG187" s="1">
+        <v>-1.7597321379076541E-13</v>
+      </c>
+      <c r="AH187" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI187" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:35">
+      <c r="A188" s="2">
+        <f>A183</f>
         <v>-2.0088544357291023E-23</v>
       </c>
-      <c r="B192">
-        <f t="shared" si="90"/>
+      <c r="B188" s="2">
+        <f t="shared" ref="B188:D188" si="92">B183</f>
         <v>3.2705030085442435E-18</v>
       </c>
-      <c r="C192">
-        <f t="shared" si="90"/>
+      <c r="C188" s="2">
+        <f t="shared" si="92"/>
         <v>-2.741905390540641E-18</v>
       </c>
-      <c r="D192">
-        <f t="shared" si="90"/>
+      <c r="D188" s="2">
+        <f t="shared" si="91"/>
+        <v>-0.41317514036883907</v>
+      </c>
+      <c r="F188" s="1"/>
+      <c r="G188" s="1"/>
+      <c r="H188" s="1"/>
+      <c r="I188" s="1">
+        <v>0</v>
+      </c>
+      <c r="J188" s="1">
+        <v>0</v>
+      </c>
+      <c r="K188" s="1">
+        <v>0</v>
+      </c>
+      <c r="L188" s="1">
+        <v>1</v>
+      </c>
+      <c r="M188" s="1"/>
+      <c r="N188" s="1">
+        <v>-2.0088544357291023E-23</v>
+      </c>
+      <c r="O188" s="1">
+        <v>3.2705030085442435E-18</v>
+      </c>
+      <c r="P188" s="1">
+        <v>-2.741905390540641E-18</v>
+      </c>
+      <c r="Q188" s="1">
+        <v>-0.41317514036883907</v>
+      </c>
+      <c r="R188" s="1"/>
+      <c r="S188" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T188" s="1">
+        <f>-O187/T186</f>
+        <v>1.8507990305124436E-13</v>
+      </c>
+      <c r="U188" s="1"/>
+      <c r="V188" s="1">
+        <v>0</v>
+      </c>
+      <c r="W188" s="1">
+        <v>0</v>
+      </c>
+      <c r="X188" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y188" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z188" s="1"/>
+      <c r="AA188" s="1">
+        <v>-2.0088544357291023E-23</v>
+      </c>
+      <c r="AB188" s="1">
+        <v>3.2705030085442435E-18</v>
+      </c>
+      <c r="AC188" s="1">
+        <v>-2.741905390540641E-18</v>
+      </c>
+      <c r="AD188" s="1">
+        <v>-0.41317514036883907</v>
+      </c>
+      <c r="AE188" s="1"/>
+      <c r="AF188" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG188" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH188" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI188" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:35">
+      <c r="A190" s="1">
+        <f t="array" ref="A190:D193">MMULT(AA185:AD188,TRANSPOSE(AF185:AI188))</f>
+        <v>-21.461131669935622</v>
+      </c>
+      <c r="B190" s="1">
+        <v>-10.917635907785833</v>
+      </c>
+      <c r="C190" s="1">
+        <v>7.5468155156407635</v>
+      </c>
+      <c r="D190" s="1">
+        <v>-1.0826114754889664</v>
+      </c>
+    </row>
+    <row r="191" spans="1:35">
+      <c r="A191" s="1">
+        <v>3.980890817081852</v>
+      </c>
+      <c r="B191" s="1">
+        <v>-12.216900138512344</v>
+      </c>
+      <c r="C191" s="1">
+        <v>-10.782789234112</v>
+      </c>
+      <c r="D191" s="1">
+        <v>-7.4229651083099206</v>
+      </c>
+    </row>
+    <row r="192" spans="1:35">
+      <c r="A192" s="1">
+        <v>-2.0164474801619994E-19</v>
+      </c>
+      <c r="B192" s="1">
+        <v>-6.5706172828686213E-20</v>
+      </c>
+      <c r="C192" s="1">
+        <v>1.160564245125121E-14</v>
+      </c>
+      <c r="D192" s="1">
+        <v>8.143970243594385</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="1">
+        <v>1.0132795648953063E-18</v>
+      </c>
+      <c r="B193" s="1">
+        <v>-3.1095746417577632E-18</v>
+      </c>
+      <c r="C193" s="1">
+        <v>-2.7419053905412165E-18</v>
+      </c>
+      <c r="D193" s="1">
+        <v>-0.41317514036883907</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
+      <c r="C194" s="1"/>
+      <c r="D194" s="1"/>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="1">
+        <f>A190+M180</f>
+        <v>-8.8736229463783207</v>
+      </c>
+      <c r="B195" s="1">
+        <f t="shared" ref="B195:D195" si="93">B190</f>
+        <v>-10.917635907785833</v>
+      </c>
+      <c r="C195" s="4">
+        <f t="shared" si="93"/>
+        <v>7.5468155156407635</v>
+      </c>
+      <c r="D195" s="4">
+        <f t="shared" si="93"/>
+        <v>-1.0826114754889664</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="1">
+        <f t="shared" ref="A196:D196" si="94">A191</f>
+        <v>3.980890817081852</v>
+      </c>
+      <c r="B196" s="1">
+        <f>B191+M180</f>
+        <v>0.3706085850449572</v>
+      </c>
+      <c r="C196" s="4">
+        <f t="shared" si="94"/>
+        <v>-10.782789234112</v>
+      </c>
+      <c r="D196" s="4">
+        <f t="shared" si="94"/>
+        <v>-7.4229651083099206</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="4">
+        <f t="shared" ref="A197:D197" si="95">A192</f>
+        <v>-2.0164474801619994E-19</v>
+      </c>
+      <c r="B197" s="4">
+        <f t="shared" si="95"/>
+        <v>-6.5706172828686213E-20</v>
+      </c>
+      <c r="C197" s="4">
+        <f>C192+M180</f>
+        <v>12.587508723557313</v>
+      </c>
+      <c r="D197" s="4">
+        <f t="shared" si="95"/>
+        <v>8.143970243594385</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="4">
+        <f t="shared" ref="A198:D198" si="96">A193</f>
+        <v>1.0132795648953063E-18</v>
+      </c>
+      <c r="B198" s="4">
+        <f t="shared" si="96"/>
+        <v>-3.1095746417577632E-18</v>
+      </c>
+      <c r="C198" s="4">
+        <f t="shared" si="96"/>
+        <v>-2.7419053905412165E-18</v>
+      </c>
+      <c r="D198" s="4">
+        <f>D193</f>
+        <v>-0.41317514036883907</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203">
+        <v>4</v>
+      </c>
+      <c r="B203">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204">
+        <f>A195</f>
+        <v>-8.8736229463783207</v>
+      </c>
+      <c r="B204">
+        <f t="shared" ref="B204:D204" si="97">B195</f>
+        <v>-10.917635907785833</v>
+      </c>
+      <c r="C204">
+        <f t="shared" si="97"/>
+        <v>7.5468155156407635</v>
+      </c>
+      <c r="D204">
+        <f t="shared" si="97"/>
+        <v>-1.0826114754889664</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205">
+        <f t="shared" ref="A205:D205" si="98">A196</f>
+        <v>3.980890817081852</v>
+      </c>
+      <c r="B205">
+        <f t="shared" si="98"/>
+        <v>0.3706085850449572</v>
+      </c>
+      <c r="C205">
+        <f t="shared" si="98"/>
+        <v>-10.782789234112</v>
+      </c>
+      <c r="D205">
+        <f t="shared" si="98"/>
+        <v>-7.4229651083099206</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206">
+        <f t="shared" ref="A206:D206" si="99">A197</f>
+        <v>-2.0164474801619994E-19</v>
+      </c>
+      <c r="B206">
+        <f t="shared" si="99"/>
+        <v>-6.5706172828686213E-20</v>
+      </c>
+      <c r="C206">
+        <f t="shared" si="99"/>
+        <v>12.587508723557313</v>
+      </c>
+      <c r="D206">
+        <f t="shared" si="99"/>
+        <v>8.143970243594385</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207">
+        <f t="shared" ref="A207:D207" si="100">A198</f>
+        <v>1.0132795648953063E-18</v>
+      </c>
+      <c r="B207">
+        <f t="shared" si="100"/>
+        <v>-3.1095746417577632E-18</v>
+      </c>
+      <c r="C207">
+        <f t="shared" si="100"/>
+        <v>-2.7419053905412165E-18</v>
+      </c>
+      <c r="D207">
+        <f t="shared" si="100"/>
         <v>-0.41317514036883907</v>
       </c>
     </row>
@@ -7153,7 +7726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A193" workbookViewId="0">
       <selection activeCell="J147" sqref="J147"/>
     </sheetView>
   </sheetViews>
@@ -15297,39 +15870,39 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3">
-        <v>12.579538945807867</v>
+        <v>-10.029677613025422</v>
       </c>
       <c r="B3">
-        <v>12.533476442090423</v>
+        <v>-7.5286908111153901</v>
       </c>
       <c r="C3">
-        <v>-8.9827134952122218</v>
+        <v>-3.8347798670194888</v>
       </c>
       <c r="E3" t="s">
         <v>39</v>
       </c>
       <c r="F3">
         <f>A3</f>
-        <v>12.579538945807867</v>
+        <v>-10.029677613025422</v>
       </c>
       <c r="H3" t="s">
         <v>40</v>
       </c>
       <c r="I3">
         <f>F3+F7+F10</f>
-        <v>4.0844943622239542</v>
+        <v>4.0844943622239533</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L3" s="1">
         <f>R9</f>
-        <v>-72.419523162995262</v>
+        <v>-72.419523162995191</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1">
         <f>L3/3</f>
-        <v>-24.139841054331754</v>
+        <v>-24.139841054331729</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -15338,44 +15911,44 @@
       </c>
       <c r="R3" s="1">
         <f>-I3</f>
-        <v>-4.0844943622239542</v>
+        <v>-4.0844943622239533</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4">
-        <v>2.3105327871348644E-2</v>
+        <v>7.3698359137508982</v>
       </c>
       <c r="B4">
-        <v>-8.3885134517630284</v>
+        <v>1.5266632516900671</v>
       </c>
       <c r="C4">
-        <v>-6.5952465187148288</v>
+        <v>12.590370584930435</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
       <c r="F4">
         <f>B3</f>
-        <v>12.533476442090423</v>
+        <v>-7.5286908111153901</v>
       </c>
       <c r="H4" t="s">
         <v>44</v>
       </c>
       <c r="I4">
         <f>F3*F7+F3*F10+F7*F10-F9*F8-F4*F6</f>
-        <v>-66.858491764648832</v>
+        <v>-66.858491764648775</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L4" s="1">
         <f>R10</f>
-        <v>-601.75672489958095</v>
+        <v>-601.75672489958106</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1">
         <f>L4/2</f>
-        <v>-300.87836244979047</v>
+        <v>-300.87836244979053</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -15384,32 +15957,32 @@
       </c>
       <c r="R4" s="1">
         <f>I4</f>
-        <v>-66.858491764648832</v>
+        <v>-66.858491764648775</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5">
-        <v>-2.2230636878927892E-20</v>
+        <v>2.1207995017926617E-19</v>
       </c>
       <c r="B5">
-        <v>5.9741822476786401</v>
+        <v>-2.3781157270230822E-12</v>
       </c>
       <c r="C5">
-        <v>-0.10653113182088469</v>
+        <v>12.587508723559308</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
       </c>
       <c r="F5">
         <f>C3</f>
-        <v>-8.9827134952122218</v>
+        <v>-3.8347798670194888</v>
       </c>
       <c r="H5" t="s">
         <v>47</v>
       </c>
       <c r="I5">
         <f>F3*F7*F10+F5*F6*F9-F3*F9*F8-F4*F6*F10</f>
-        <v>505.68145814092458</v>
+        <v>505.68145814092486</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -15422,7 +15995,7 @@
       </c>
       <c r="R5" s="1">
         <f>-I5</f>
-        <v>-505.68145814092458</v>
+        <v>-505.68145814092486</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -15431,21 +16004,21 @@
       </c>
       <c r="F6">
         <f>A4</f>
-        <v>2.3105327871348644E-2</v>
+        <v>7.3698359137508982</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L6" s="1">
         <f>-L4/2</f>
-        <v>300.87836244979047</v>
+        <v>300.87836244979053</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="N6" s="1">
         <f>L4*L4/4 + L3*L3*L3/27</f>
-        <v>76460.732916443289</v>
+        <v>76460.732916443376</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>52</v>
@@ -15460,21 +16033,21 @@
       </c>
       <c r="F7">
         <f>B4</f>
-        <v>-8.3885134517630284</v>
+        <v>1.5266632516900671</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="L7" s="1">
         <f>L6</f>
-        <v>300.87836244979047</v>
+        <v>300.87836244979053</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>55</v>
       </c>
       <c r="N7" s="1">
         <f>N6</f>
-        <v>76460.732916443289</v>
+        <v>76460.732916443376</v>
       </c>
       <c r="O7" s="1" t="str">
         <f>O6</f>
@@ -15486,7 +16059,7 @@
       </c>
       <c r="R7" s="1">
         <f>-R3/3</f>
-        <v>1.3614981207413182</v>
+        <v>1.3614981207413177</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -15495,7 +16068,7 @@
       </c>
       <c r="F8">
         <f>C4</f>
-        <v>-6.5952465187148288</v>
+        <v>12.590370584930435</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -15512,7 +16085,7 @@
       </c>
       <c r="F9">
         <f>B5</f>
-        <v>5.9741822476786401</v>
+        <v>-2.3781157270230822E-12</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>59</v>
@@ -15530,7 +16103,7 @@
       </c>
       <c r="R9" s="1">
         <f>3*R7*R7+2*R3*R7+R4</f>
-        <v>-72.419523162995262</v>
+        <v>-72.419523162995191</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -15539,14 +16112,14 @@
       </c>
       <c r="F10">
         <f>C5</f>
-        <v>-0.10653113182088469</v>
+        <v>12.587508723559308</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="L10" s="1">
         <f>POWER(L7-SQRT(N7), 1/3)</f>
-        <v>2.8989700291054201</v>
+        <v>2.8989700291054157</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -15557,7 +16130,7 @@
       </c>
       <c r="R10" s="1">
         <f>R7*R7*R7+R3*R7*R7+R4*R7+R5</f>
-        <v>-601.75672489958095</v>
+        <v>-601.75672489958106</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -15576,7 +16149,7 @@
       </c>
       <c r="L12" s="1">
         <f>L9+L10</f>
-        <v>11.226010602815997</v>
+        <v>11.226010602815991</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -15587,7 +16160,7 @@
       </c>
       <c r="R12" s="1">
         <f>L12+R7</f>
-        <v>12.587508723557315</v>
+        <v>12.58750872355731</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -15633,7 +16206,7 @@
       </c>
       <c r="L16" s="1">
         <f>SQRT(L6*L6+ABS(N6))</f>
-        <v>408.64229089377272</v>
+        <v>408.64229089377289</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="s">
@@ -15641,7 +16214,7 @@
       </c>
       <c r="O16" s="1">
         <f>SQRT(-L3/3)</f>
-        <v>4.9132312233734483</v>
+        <v>4.9132312233734456</v>
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -15740,31 +16313,31 @@
     <row r="24" spans="1:33">
       <c r="A24">
         <f>A3-R12</f>
-        <v>-7.9697777494480704E-3</v>
+        <v>-22.617186336582733</v>
       </c>
       <c r="B24">
         <f t="shared" ref="B24:C24" si="0">B3</f>
-        <v>12.533476442090423</v>
+        <v>-7.5286908111153901</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>-8.9827134952122218</v>
+        <v>-3.8347798670194888</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F24" s="1">
         <f>SQRT(A24*A24+A25*A25)</f>
-        <v>2.4441226103003057E-2</v>
+        <v>23.787635426399934</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1">
         <f>F25</f>
-        <v>-0.326079293888977</v>
+        <v>-0.95079590430757088</v>
       </c>
       <c r="I24" s="1">
         <f>-F26</f>
-        <v>0.94534242161074422</v>
+        <v>0.30981792774458472</v>
       </c>
       <c r="J24" s="1">
         <v>0</v>
@@ -15772,13 +16345,13 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1">
         <f t="array" ref="L24:N26">MMULT(H24:J26,A24:C26)</f>
-        <v>2.4441226103003057E-2</v>
+        <v>23.787635426399937</v>
       </c>
       <c r="M24" s="1">
-        <v>-23.916430747188979</v>
+        <v>3.7314001648095747</v>
       </c>
       <c r="N24" s="1">
-        <v>-3.3056894413959212</v>
+        <v>7.5468155156427841</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1" t="s">
@@ -15786,7 +16359,7 @@
       </c>
       <c r="Q24" s="1">
         <f>SQRT(M25*M25+M26*M26)</f>
-        <v>7.7959432955453618</v>
+        <v>12.849129958559782</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1">
@@ -15801,77 +16374,77 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1">
         <f t="array" ref="W24:Y26">MMULT(S24:U26,L24:N26)</f>
-        <v>2.4441226103003057E-2</v>
+        <v>23.787635426399937</v>
       </c>
       <c r="X24" s="1">
-        <v>-23.916430747188979</v>
+        <v>3.7314001648095747</v>
       </c>
       <c r="Y24" s="1">
-        <v>-3.3056894413959212</v>
+        <v>7.5468155156427841</v>
       </c>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1">
         <f t="array" ref="AA24:AC26">MMULT(W24:Y26,TRANSPOSE(H24:J26))</f>
-        <v>-22.617186336582737</v>
+        <v>-21.461131669935632</v>
       </c>
       <c r="AB24" s="1">
-        <v>7.7755475225166517</v>
+        <v>-10.917635907784438</v>
       </c>
       <c r="AC24" s="1">
-        <v>-3.3056894413959212</v>
+        <v>7.5468155156427841</v>
       </c>
       <c r="AE24" s="1">
         <f t="array" ref="AE24:AG26">MMULT(AA24:AC26,TRANSPOSE(S24:U26))</f>
-        <v>-22.617186336582737</v>
+        <v>-21.461131669935632</v>
       </c>
       <c r="AF24" s="1">
-        <v>-7.5286908111153901</v>
+        <v>-10.917635907785835</v>
       </c>
       <c r="AG24" s="1">
-        <v>-3.8347798670194897</v>
+        <v>7.5468155156407635</v>
       </c>
     </row>
     <row r="25" spans="1:33">
       <c r="A25">
         <f t="shared" ref="A25:C26" si="1">A4</f>
-        <v>2.3105327871348644E-2</v>
+        <v>7.3698359137508982</v>
       </c>
       <c r="B25">
         <f>B4-R12</f>
-        <v>-20.976022175320345</v>
+        <v>-11.060845471867243</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>-6.5952465187148288</v>
+        <v>12.590370584930435</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F25" s="1">
         <f>A24/F24</f>
-        <v>-0.326079293888977</v>
+        <v>-0.95079590430757088</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1">
         <f>F26</f>
-        <v>-0.94534242161074422</v>
+        <v>-0.30981792774458472</v>
       </c>
       <c r="I25" s="1">
         <f>F25</f>
-        <v>-0.326079293888977</v>
+        <v>-0.95079590430757088</v>
       </c>
       <c r="J25" s="1">
         <v>0</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1">
-        <v>8.6736173798840355E-19</v>
+        <v>-8.8817841970012523E-16</v>
       </c>
       <c r="M25" s="1">
-        <v>-5.0085804714389948</v>
+        <v>12.849129958559782</v>
       </c>
       <c r="N25" s="1">
-        <v>10.642313456045699</v>
+        <v>-10.782789234109741</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
@@ -15879,7 +16452,7 @@
       </c>
       <c r="Q25" s="1">
         <f>M25/Q24</f>
-        <v>-0.64245983860617883</v>
+        <v>1</v>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1">
@@ -15887,61 +16460,61 @@
       </c>
       <c r="T25" s="1">
         <f>Q25</f>
-        <v>-0.64245983860617883</v>
+        <v>1</v>
       </c>
       <c r="U25" s="1">
         <f>-Q26</f>
-        <v>0.76631935625959668</v>
+        <v>-1.8507990305124423E-13</v>
       </c>
       <c r="V25" s="1"/>
       <c r="W25" s="1">
-        <v>-5.7428084954350538E-19</v>
+        <v>-8.8817841970012523E-16</v>
       </c>
       <c r="X25" s="1">
-        <v>7.7959432955453618</v>
+        <v>12.849129958559782</v>
       </c>
       <c r="Y25" s="1">
-        <v>-16.564947435674572</v>
+        <v>-10.782789234109741</v>
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1">
-        <v>7.3698359137508982</v>
+        <v>3.9808908170818542</v>
       </c>
       <c r="AB25" s="1">
-        <v>-2.5420956850099357</v>
+        <v>-12.216900138514349</v>
       </c>
       <c r="AC25" s="1">
-        <v>-16.564947435674572</v>
+        <v>-10.782789234109741</v>
       </c>
       <c r="AE25" s="1">
-        <v>7.3698359137508982</v>
+        <v>3.9808908170818542</v>
       </c>
       <c r="AF25" s="1">
-        <v>-11.060845471867248</v>
+        <v>-12.216900138512354</v>
       </c>
       <c r="AG25" s="1">
-        <v>12.590370584930435</v>
+        <v>-10.782789234112002</v>
       </c>
     </row>
     <row r="26" spans="1:33">
       <c r="A26">
         <f t="shared" si="1"/>
-        <v>-2.2230636878927892E-20</v>
+        <v>2.1207995017926617E-19</v>
       </c>
       <c r="B26">
         <f t="shared" si="1"/>
-        <v>5.9741822476786401</v>
+        <v>-2.3781157270230822E-12</v>
       </c>
       <c r="C26">
         <f>C5-R12</f>
-        <v>-12.6940398553782</v>
+        <v>1.9984014443252818E-12</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F26" s="1">
         <f>-A25/F24</f>
-        <v>-0.94534242161074422</v>
+        <v>-0.30981792774458472</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1">
@@ -15955,13 +16528,13 @@
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1">
-        <v>-2.2230636878927892E-20</v>
+        <v>2.1207995017926617E-19</v>
       </c>
       <c r="M26" s="1">
-        <v>5.9741822476786401</v>
+        <v>-2.3781157270230822E-12</v>
       </c>
       <c r="N26" s="1">
-        <v>-12.6940398553782</v>
+        <v>1.9984014443252818E-12</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1" t="s">
@@ -15969,7 +16542,7 @@
       </c>
       <c r="Q26" s="1">
         <f>-M26/Q24</f>
-        <v>-0.76631935625959668</v>
+        <v>1.8507990305124423E-13</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1">
@@ -15977,40 +16550,40 @@
       </c>
       <c r="T26" s="1">
         <f>Q26</f>
-        <v>-0.76631935625959668</v>
+        <v>1.8507990305124423E-13</v>
       </c>
       <c r="U26" s="1">
         <f>Q25</f>
-        <v>-0.64245983860617883</v>
+        <v>1</v>
       </c>
       <c r="V26" s="1"/>
       <c r="W26" s="1">
-        <v>-6.5039379731812975E-19</v>
+        <v>2.120799500148822E-19</v>
       </c>
       <c r="X26" s="1">
         <v>0</v>
       </c>
       <c r="Y26" s="1">
-        <v>-3.1032953984322376E-12</v>
+        <v>2.7238582542507655E-15</v>
       </c>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1">
-        <v>2.1207995017926617E-19</v>
+        <v>-2.0164474785990435E-19</v>
       </c>
       <c r="AB26" s="1">
-        <v>6.1484484735732833E-19</v>
+        <v>-6.5706170629785912E-20</v>
       </c>
       <c r="AC26" s="1">
-        <v>-3.1032953984322376E-12</v>
+        <v>2.7238582542507655E-15</v>
       </c>
       <c r="AE26" s="1">
-        <v>2.1207995017926617E-19</v>
+        <v>-2.0164474785990435E-19</v>
       </c>
       <c r="AF26" s="1">
-        <v>-2.3781157270230822E-12</v>
+        <v>-6.5706171133917335E-20</v>
       </c>
       <c r="AG26" s="1">
-        <v>1.9937421896565653E-12</v>
+        <v>2.7238582542507655E-15</v>
       </c>
     </row>
     <row r="28" spans="1:33">
@@ -16029,47 +16602,48 @@
     <row r="30" spans="1:33">
       <c r="A30">
         <f>AE24+R12</f>
-        <v>-10.029677613025422</v>
+        <v>-8.8736229463783225</v>
       </c>
       <c r="B30">
         <f t="shared" ref="B30:C31" si="2">AF24</f>
-        <v>-7.5286908111153901</v>
+        <v>-10.917635907785835</v>
       </c>
       <c r="C30">
         <f t="shared" si="2"/>
-        <v>-3.8347798670194897</v>
+        <v>7.5468155156407635</v>
       </c>
     </row>
     <row r="31" spans="1:33">
       <c r="A31">
         <f t="shared" ref="A31:B32" si="3">AE25</f>
-        <v>7.3698359137508982</v>
+        <v>3.9808908170818542</v>
       </c>
       <c r="B31">
         <f>AF25+R12</f>
-        <v>1.5266632516900671</v>
+        <v>0.37060858504495542</v>
       </c>
       <c r="C31">
         <f t="shared" si="2"/>
-        <v>12.590370584930435</v>
+        <v>-10.782789234112002</v>
       </c>
     </row>
     <row r="32" spans="1:33">
       <c r="A32">
         <f t="shared" si="3"/>
-        <v>2.1207995017926617E-19</v>
+        <v>-2.0164474785990435E-19</v>
       </c>
       <c r="B32">
         <f t="shared" si="3"/>
-        <v>-2.3781157270230822E-12</v>
+        <v>-6.5706171133917335E-20</v>
       </c>
       <c r="C32">
         <f>AG26+R12</f>
-        <v>12.587508723559308</v>
+        <v>12.587508723557313</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17434,545 +18008,545 @@
     <row r="1" spans="1:8">
       <c r="A1">
         <f ca="1">RAND()*20-7</f>
-        <v>7.9094871569319274</v>
+        <v>7.8068931460313067</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:H16" ca="1" si="0">RAND()*20-7</f>
-        <v>-2.2138207610073568</v>
+        <v>-5.4218868755512677</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16392628576887791</v>
+        <v>1.4707881960181037</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4807129580119121</v>
+        <v>5.4993735121968115</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8454269769969489</v>
+        <v>10.14354485556688</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.952305541618887</v>
+        <v>7.5703138067299971</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6879569056033894</v>
+        <v>3.7669478209825265</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3220788411567739</v>
+        <v>-5.2218415948237151</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
         <f t="shared" ref="A2:A16" ca="1" si="1">RAND()*20-7</f>
-        <v>7.154616651938877</v>
+        <v>11.861017606170382</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.0722813057663281</v>
+        <v>3.4101152247394459</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8589355750185828</v>
+        <v>6.7107778580434747</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8104309583642326</v>
+        <v>0.64650180854225869</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>11.903907712216387</v>
+        <v>-5.2831941032591372</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4704604973111639</v>
+        <v>-3.1914165565794388</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>11.06795579635471</v>
+        <v>8.4149564942070487</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6114264462145353</v>
+        <v>5.5590730125038252</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9441788242987919</v>
+        <v>10.286388597524734</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.8455801347462124</v>
+        <v>8.5661216214055287</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.4161400049883168</v>
+        <v>-4.6250188492194715</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6702013298754519</v>
+        <v>5.0970788286865378</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43812295381335975</v>
+        <v>6.6005028242037653</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>10.760374468124951</v>
+        <v>10.602935434617951</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4566905808556925</v>
+        <v>-1.1473272986431597</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.202985067324585</v>
+        <v>8.0227367713805471</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5365652893755701</v>
+        <v>6.0499396077615408</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.53512826343225406</v>
+        <v>3.4032899855038252</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.9371992612388489</v>
+        <v>0.22420659621348271</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1057418654362507</v>
+        <v>-1.0015343593731423</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>10.168637744740472</v>
+        <v>12.855936950266269</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>12.991727240962906</v>
+        <v>11.88205329363856</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>12.937610113847718</v>
+        <v>7.0957785569422462</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.116145855941995</v>
+        <v>1.5720021148277681</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.2122666397695658</v>
+        <v>10.515714368933814</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.3759592070820794</v>
+        <v>9.8093159103015282</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30874508448758231</v>
+        <v>-3.6291322009191744</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5059877810292868</v>
+        <v>-6.4880786441451992</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6432924810681975</v>
+        <v>6.2500795325949046</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>12.863566082160688</v>
+        <v>5.6539943065458758</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.3994729453746464</v>
+        <v>6.7045731162685662</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.3563140236218283</v>
+        <v>-4.0479669645668857</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1474042697163096</v>
+        <v>10.514467906995446</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>11.883926417586459</v>
+        <v>0.97176530531841188</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5290794490463497E-2</v>
+        <v>-2.7244651064227821</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.8234523684380326</v>
+        <v>4.8472594473352526</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5634531803317788</v>
+        <v>-4.7175200587772386</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8785691191847578</v>
+        <v>6.2073427694431338</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2250903913058711</v>
+        <v>0.15921301942659305</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0889148392602852</v>
+        <v>1.3161010010811545</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.0707743800545648</v>
+        <v>-6.1034901592017636</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>11.915886062787262</v>
+        <v>-6.5619303906866682</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9504137569228766</v>
+        <v>9.494499729150899</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6870951421601834</v>
+        <v>-0.69135479217802143</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1521695485011536</v>
+        <v>10.387022391997672</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4098922805332847</v>
+        <v>-3.9044477867348819</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.613538162077941</v>
+        <v>9.6795679035147444</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4842832446064449</v>
+        <v>-0.33976066007312511</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.0210300772528171</v>
+        <v>-6.3692856959867843</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.9767924811918114</v>
+        <v>1.5946949890908755</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2157914216620114</v>
+        <v>3.8414418949944569</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.3263856817163582</v>
+        <v>8.9307210996976742</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1908344620440214</v>
+        <v>10.206436539656231</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.79433298462935653</v>
+        <v>-4.9591594548558557</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>12.301604438475227</v>
+        <v>-0.28118132430479115</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>12.263878671103846</v>
+        <v>2.4022250006632735</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0931796125932998</v>
+        <v>0.12651646453267507</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5986783052002451</v>
+        <v>11.93318563929579</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5016621816982987</v>
+        <v>1.5244662140014178</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>12.800182717716236</v>
+        <v>-6.4973074079832358</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6708079719297277</v>
+        <v>10.477120789113158</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>10.313852551123947</v>
+        <v>4.512739922161682</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>10.161431639908223</v>
+        <v>11.408477509917866</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.5673860846408783</v>
+        <v>0.57074699117446848</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>12.321981689606158</v>
+        <v>7.2205064865981985</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2979819208274197</v>
+        <v>-6.6050285289770247</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7895414875692985</v>
+        <v>9.2282973961709516</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7579705126006289E-3</v>
+        <v>0.49645598949241254</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1966783338395288</v>
+        <v>-2.6660209788354932</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.9156939925415806</v>
+        <v>9.1294319853451249</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6675013499417517</v>
+        <v>4.9443234080213667</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8900172858018891</v>
+        <v>-3.0255143319499083</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.4874203486113413</v>
+        <v>9.4050545804718411</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2868373843883401</v>
+        <v>6.2985004745626263</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.7940239705538836</v>
+        <v>2.5541050297198105</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>10.557329688700356</v>
+        <v>-3.5264977219358844</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7849322678626613</v>
+        <v>6.1847949653047856</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9963443354403525</v>
+        <v>7.7925041490684883</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.8846533745928093</v>
+        <v>3.3531830078916887</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>12.501224931171734</v>
+        <v>1.9688912496429403</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.8330515491554982</v>
+        <v>11.21153172787432</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7517097451064814</v>
+        <v>-4.8085882755765024</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.8698550989101141</v>
+        <v>10.755254056238787</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4235917077335305</v>
+        <v>-4.8533534655537585</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6695703985156456</v>
+        <v>9.6199274563292967</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3656712408824934</v>
+        <v>-2.220946647631024</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.543033394831042</v>
+        <v>4.3605278029573924</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2118278029925555</v>
+        <v>-1.8589485034460971</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6165361143597092</v>
+        <v>1.3165879646185576</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>10.979414162129473</v>
+        <v>0.54396091019212012</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.3028896373085743</v>
+        <v>12.54171322189779</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8613306903397469</v>
+        <v>12.845557694282668</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2709419340851493</v>
+        <v>0.68637677626997373</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5587063564986607</v>
+        <v>11.064650986471122</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>10.622747210037215</v>
+        <v>-0.67848992495319038</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1431560397569793</v>
+        <v>6.2562005397492833</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4129087787761261</v>
+        <v>5.4435087811790712</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7636084599836916</v>
+        <v>-5.7721337947420324</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8316830352906344</v>
+        <v>-2.7724297078090059</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8719301355950062</v>
+        <v>-2.8702672454893339</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3981668764028452</v>
+        <v>10.34370984578036</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7768070380842502</v>
+        <v>-1.5864192307689544</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0390050263302388</v>
+        <v>2.7086381241617214</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1839134187863944</v>
+        <v>-5.5684912638731925</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6149315603464398</v>
+        <v>9.6046865587843158</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.2387170381038928</v>
+        <v>9.2546203132204887</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48991898253817112</v>
+        <v>2.6450054933916221</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1440092509603774</v>
+        <v>5.0525152090039551</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5025844029578561</v>
+        <v>1.2110691547495822</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.605404378478763</v>
+        <v>7.2147624447350669</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28932268624851787</v>
+        <v>-0.55748955338555817</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4430537508880228</v>
+        <v>3.103392542729047</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>12.81497037526999</v>
+        <v>-0.13270669665383927</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94359261929781724</v>
+        <v>10.836006245635282</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6364329218515579</v>
+        <v>-1.1018954561118592</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>11.946267378849175</v>
+        <v>-5.0911688139730531</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3435110876448757</v>
+        <v>4.1362543169801587</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>10.173089344657097</v>
+        <v>12.567506077075411</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>12.352980591162037</v>
+        <v>10.155997009693117</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.348361589264508</v>
+        <v>-0.23910156072264588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>